<commit_message>
add browsercontrol and implement page object model
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="5640"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -377,7 +377,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
add util keywords and common class
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="5640"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="5640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="FilterProduct" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>pageheader</t>
+  </si>
+  <si>
+    <t>Swag Labs</t>
+  </si>
+  <si>
+    <t>filterproduct</t>
+  </si>
+  <si>
+    <t>Price (low to high)</t>
   </si>
 </sst>
 </file>
@@ -374,68 +386,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -446,12 +479,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>